<commit_message>
Updated graph axes thickness
</commit_message>
<xml_diff>
--- a/StateOfPractice/DomainMeasurements/LBM-Peter/Report/LBM_Figures_Updated_01OCT2022.xlsx
+++ b/StateOfPractice/DomainMeasurements/LBM-Peter/Report/LBM_Figures_Updated_01OCT2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smiths/Repos/AIMSS/StateOfPractice/DomainMeasurements/LBM-Peter/Report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD97D606-D598-6848-B73B-A71F472DAAE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7180F351-61BF-7440-8B48-3A481A84982F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19580" yWindow="2280" windowWidth="26620" windowHeight="16860" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19580" yWindow="2280" windowWidth="26620" windowHeight="16860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -552,7 +552,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-CA" sz="900" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -576,7 +576,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -883,7 +883,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -958,7 +958,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -1650,7 +1650,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -1726,7 +1726,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -2033,7 +2033,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -2084,7 +2084,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-CA" sz="900" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2108,7 +2108,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -2415,7 +2415,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -2467,7 +2467,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-CA" sz="900" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2491,7 +2491,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -2799,7 +2799,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -2849,7 +2849,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-CA" sz="900" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -2873,7 +2873,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -3181,7 +3181,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -3231,7 +3231,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-CA" sz="900" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -3255,7 +3255,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -3563,7 +3563,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -3613,7 +3613,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-CA" sz="900" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -3637,7 +3637,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -3944,7 +3944,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -3994,7 +3994,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="1" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-CA" sz="900" b="1" strike="noStrike" spc="-1">
                     <a:solidFill>
                       <a:srgbClr val="000000"/>
                     </a:solidFill>
@@ -4018,7 +4018,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
-          <a:ln w="0">
+          <a:ln w="15875">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -4080,8 +4080,8 @@
       <xdr:rowOff>143640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>783000</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>15875</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
@@ -4121,8 +4121,8 @@
       <xdr:rowOff>121680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>792720</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>121680</xdr:rowOff>
     </xdr:to>
@@ -4197,16 +4197,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>799560</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>21685</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>55440</xdr:rowOff>
+      <xdr:rowOff>23690</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>802800</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>13610</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4244,8 +4244,8 @@
       <xdr:rowOff>17280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>802800</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>857250</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>157680</xdr:rowOff>
     </xdr:to>
@@ -4280,13 +4280,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>6480</xdr:colOff>
+      <xdr:colOff>6479</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>26280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>792720</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>15874</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>134640</xdr:rowOff>
     </xdr:to>
@@ -4321,13 +4321,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>26280</xdr:colOff>
+      <xdr:colOff>26279</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>55080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>802800</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>857249</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>42480</xdr:rowOff>
     </xdr:to>
@@ -4367,8 +4367,8 @@
       <xdr:rowOff>26640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>783000</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>17280</xdr:rowOff>
     </xdr:to>
@@ -4408,8 +4408,8 @@
       <xdr:rowOff>141120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>802800</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>109080</xdr:rowOff>
     </xdr:to>
@@ -4449,8 +4449,8 @@
       <xdr:rowOff>102600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>802800</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>83160</xdr:rowOff>
     </xdr:to>
@@ -4779,8 +4779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R34" sqref="R34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4993,7 +4993,7 @@
   <dimension ref="A2:B25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+      <selection activeCell="R39" sqref="R39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5205,8 +5205,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:B25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5418,8 +5418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -5844,7 +5844,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:B25"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
@@ -6058,7 +6058,7 @@
   <dimension ref="A2:B25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6271,7 +6271,7 @@
   <dimension ref="A2:B25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6484,7 +6484,7 @@
   <dimension ref="A2:B25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6697,7 +6697,7 @@
   <dimension ref="A2:B25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>